<commit_message>
water quality data and biodiversity data input
</commit_message>
<xml_diff>
--- a/prep/SPP/marine_mammals_ESA_status.xlsx
+++ b/prep/SPP/marine_mammals_ESA_status.xlsx
@@ -16,16 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
-  <si>
-    <t>species</t>
-  </si>
-  <si>
-    <t>habitat_extent</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="71">
   <si>
     <t>E</t>
   </si>
@@ -33,62 +24,230 @@
     <t>NC</t>
   </si>
   <si>
-    <t>rgn_id</t>
-  </si>
-  <si>
     <t>Stenella longirostris longirostris)</t>
   </si>
   <si>
-    <t>strategic</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>Risso's</t>
-  </si>
-  <si>
     <t>Grampus griseus</t>
   </si>
   <si>
-    <t>commmon</t>
-  </si>
-  <si>
-    <t>Frazers</t>
-  </si>
-  <si>
-    <t>Common Bottlenose Dolphin</t>
-  </si>
-  <si>
     <t>Tursiops truncatus truncatus</t>
   </si>
   <si>
     <t>Stenella attenuata attenuata</t>
   </si>
   <si>
-    <t>Pantropical Spotted Dolphin</t>
-  </si>
-  <si>
-    <t>Spinner Dolphin</t>
-  </si>
-  <si>
-    <t>Grey Whale</t>
-  </si>
-  <si>
-    <t>Humpback Whale</t>
+    <t>Humpback whale</t>
+  </si>
+  <si>
+    <t>Short-finned pilot whale</t>
+  </si>
+  <si>
+    <t>Pantropical spotted dolphin</t>
+  </si>
+  <si>
+    <t>Common bottlenose dolphin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rough-toothed dolphin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spinner dolphin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sperm whale </t>
+  </si>
+  <si>
+    <t>Cuvier’s beaked whale</t>
+  </si>
+  <si>
+    <t>Dwarf sperm whale</t>
+  </si>
+  <si>
+    <t>False killer whale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melon-headed whale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Striped dolphin </t>
+  </si>
+  <si>
+    <t>Blainville’s beaked whale</t>
+  </si>
+  <si>
+    <t>Pygmy killer whale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Risso’s dolphin </t>
+  </si>
+  <si>
+    <t>Pygmy sperm whale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bryde’s whale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sei whale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Killer whale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraser’s dolphin </t>
+  </si>
+  <si>
+    <t>Longman’s beaked whale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fin whale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minke whale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue whale </t>
+  </si>
+  <si>
+    <t>Common name</t>
+  </si>
+  <si>
+    <t>ESA Status</t>
+  </si>
+  <si>
+    <t>IUCN status</t>
+  </si>
+  <si>
+    <t>Loggerhead</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Leatherback</t>
+  </si>
+  <si>
+    <t>Hawksbill</t>
+  </si>
+  <si>
+    <t>Olive Ridley</t>
+  </si>
+  <si>
+    <t>Caretta caretta</t>
+  </si>
+  <si>
+    <t>Chelonia mydas</t>
+  </si>
+  <si>
+    <t>Dermochelys cariacea</t>
+  </si>
+  <si>
+    <t>Ertmochelys imbricata</t>
+  </si>
+  <si>
+    <t>Lepidochelys olivacea</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Species name</t>
+  </si>
+  <si>
+    <t>Balaenoptera musculus musculus</t>
+  </si>
+  <si>
+    <t>Balaenoptera edeni</t>
+  </si>
+  <si>
+    <t>Balaenoptera physalus physalus</t>
+  </si>
+  <si>
+    <t>Balaenoptera acutorostrata scammoni</t>
+  </si>
+  <si>
+    <t>Balaenoptera borealis borealis</t>
+  </si>
+  <si>
+    <t>Physeter macrocephalus</t>
+  </si>
+  <si>
+    <t>Lagenodelphis hosei</t>
+  </si>
+  <si>
+    <t>Lissodelphis borealis</t>
+  </si>
+  <si>
+    <t>Steno bredanensis</t>
+  </si>
+  <si>
+    <t>Stenella coeruleoalba</t>
+  </si>
+  <si>
+    <t>Mesoplodon densirostris</t>
+  </si>
+  <si>
+    <t>Ziphius cavirostris</t>
+  </si>
+  <si>
+    <t>Kogia sima</t>
+  </si>
+  <si>
+    <t>Pseudorca crassidens</t>
+  </si>
+  <si>
+    <t>Orcinus orca</t>
+  </si>
+  <si>
+    <t>Peponocephala electra</t>
+  </si>
+  <si>
+    <t>Globicephala macrorhynchus</t>
+  </si>
+  <si>
+    <t>Feresa attenuata</t>
+  </si>
+  <si>
+    <t>Kogia breviceps</t>
+  </si>
+  <si>
+    <t>Neomonachus schauinslandi</t>
+  </si>
+  <si>
+    <t>Hawaiian monk seal</t>
+  </si>
+  <si>
+    <t>Indopacetus pacificus</t>
+  </si>
+  <si>
+    <t>Megaptera novaeangliae</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Not considered depleted or a species of concern in Hawaii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Pacific right </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,7 +258,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -107,12 +266,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,111 +597,388 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="3" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C23" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="C31" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
+      <c r="B32" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P32" s="1"/>
     </row>
   </sheetData>
+  <sortState ref="A2:G32">
+    <sortCondition ref="A2:A32"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>